<commit_message>
All of 20201007 Egg Bundle Counts
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Oct_2020/Wild_vs_Nurs/Eggs.per.bundle.xlsx
+++ b/RAnalysis/Data/Oct_2020/Wild_vs_Nurs/Eggs.per.bundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcone\Documents\URI\Lab-Notebook\Apul_Spawning_Nurs.vs.Wild\RAnalysis\Data\Oct_2020\Wild_vs_Nurs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266FD44-567D-4D10-A476-068D9E1A644E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDED184C-8735-4AEF-B644-5D46C1EFA7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12D853DE-AEAC-4013-830B-575094CDB5AA}"/>
   </bookViews>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22587122-F93A-462F-9056-C7037AE0927B}">
   <dimension ref="A1:I385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A369" workbookViewId="0">
-      <selection activeCell="E391" sqref="E391"/>
+    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
+      <selection activeCell="G386" sqref="G386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6069,6 +6069,9 @@
       <c r="F242">
         <v>1</v>
       </c>
+      <c r="G242">
+        <v>6</v>
+      </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
@@ -6089,6 +6092,9 @@
       <c r="F243">
         <v>2</v>
       </c>
+      <c r="G243">
+        <v>6</v>
+      </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
@@ -6109,6 +6115,9 @@
       <c r="F244">
         <v>3</v>
       </c>
+      <c r="G244">
+        <v>8</v>
+      </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
@@ -6129,6 +6138,9 @@
       <c r="F245">
         <v>4</v>
       </c>
+      <c r="G245">
+        <v>5</v>
+      </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
@@ -6149,6 +6161,9 @@
       <c r="F246">
         <v>5</v>
       </c>
+      <c r="G246">
+        <v>8</v>
+      </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
@@ -6169,6 +6184,9 @@
       <c r="F247">
         <v>6</v>
       </c>
+      <c r="G247">
+        <v>4</v>
+      </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
@@ -6189,6 +6207,9 @@
       <c r="F248">
         <v>7</v>
       </c>
+      <c r="G248">
+        <v>7</v>
+      </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
@@ -6209,6 +6230,9 @@
       <c r="F249">
         <v>8</v>
       </c>
+      <c r="G249">
+        <v>4</v>
+      </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
@@ -6229,6 +6253,9 @@
       <c r="F250">
         <v>9</v>
       </c>
+      <c r="G250">
+        <v>5</v>
+      </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
@@ -6249,6 +6276,9 @@
       <c r="F251">
         <v>10</v>
       </c>
+      <c r="G251">
+        <v>10</v>
+      </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
@@ -6269,6 +6299,9 @@
       <c r="F252">
         <v>11</v>
       </c>
+      <c r="G252">
+        <v>3</v>
+      </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253">
@@ -6289,6 +6322,9 @@
       <c r="F253">
         <v>12</v>
       </c>
+      <c r="G253">
+        <v>7</v>
+      </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254">
@@ -6309,6 +6345,9 @@
       <c r="F254">
         <v>13</v>
       </c>
+      <c r="G254">
+        <v>10</v>
+      </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255">
@@ -6329,6 +6368,9 @@
       <c r="F255">
         <v>14</v>
       </c>
+      <c r="G255">
+        <v>4</v>
+      </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256">
@@ -6349,8 +6391,11 @@
       <c r="F256">
         <v>15</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G256">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>20201007</v>
       </c>
@@ -6369,8 +6414,11 @@
       <c r="F257">
         <v>16</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G257">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>20201007</v>
       </c>
@@ -6389,8 +6437,11 @@
       <c r="F258">
         <v>17</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G258">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>20201007</v>
       </c>
@@ -6409,8 +6460,11 @@
       <c r="F259">
         <v>18</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G259">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>20201007</v>
       </c>
@@ -6429,8 +6483,11 @@
       <c r="F260">
         <v>19</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G260">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>20201007</v>
       </c>
@@ -6449,8 +6506,11 @@
       <c r="F261">
         <v>20</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G261">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>20201007</v>
       </c>
@@ -6469,8 +6529,11 @@
       <c r="F262">
         <v>21</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G262">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>20201007</v>
       </c>
@@ -6489,8 +6552,11 @@
       <c r="F263">
         <v>22</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G263">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>20201007</v>
       </c>
@@ -6509,8 +6575,11 @@
       <c r="F264">
         <v>23</v>
       </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G264">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>20201007</v>
       </c>
@@ -6529,8 +6598,11 @@
       <c r="F265">
         <v>24</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>20201007</v>
       </c>
@@ -6549,8 +6621,11 @@
       <c r="F266">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G266">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>20201007</v>
       </c>
@@ -6569,8 +6644,11 @@
       <c r="F267">
         <v>2</v>
       </c>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G267">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>20201007</v>
       </c>
@@ -6589,8 +6667,11 @@
       <c r="F268">
         <v>3</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G268">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>20201007</v>
       </c>
@@ -6609,8 +6690,11 @@
       <c r="F269">
         <v>4</v>
       </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G269">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>20201007</v>
       </c>
@@ -6629,8 +6713,11 @@
       <c r="F270">
         <v>5</v>
       </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>20201007</v>
       </c>
@@ -6649,8 +6736,11 @@
       <c r="F271">
         <v>6</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G271">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>20201007</v>
       </c>
@@ -6669,8 +6759,11 @@
       <c r="F272">
         <v>7</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G272">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>20201007</v>
       </c>
@@ -6689,8 +6782,11 @@
       <c r="F273">
         <v>8</v>
       </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G273">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>20201007</v>
       </c>
@@ -6709,8 +6805,11 @@
       <c r="F274">
         <v>9</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G274">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>20201007</v>
       </c>
@@ -6729,8 +6828,11 @@
       <c r="F275">
         <v>10</v>
       </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G275">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>20201007</v>
       </c>
@@ -6749,8 +6851,11 @@
       <c r="F276">
         <v>11</v>
       </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G276">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>20201007</v>
       </c>
@@ -6769,8 +6874,11 @@
       <c r="F277">
         <v>12</v>
       </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G277">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>20201007</v>
       </c>
@@ -6789,8 +6897,11 @@
       <c r="F278">
         <v>13</v>
       </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G278">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>20201007</v>
       </c>
@@ -6809,8 +6920,11 @@
       <c r="F279">
         <v>14</v>
       </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G279">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>20201007</v>
       </c>
@@ -6829,8 +6943,11 @@
       <c r="F280">
         <v>15</v>
       </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>20201007</v>
       </c>
@@ -6849,8 +6966,11 @@
       <c r="F281">
         <v>16</v>
       </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G281">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>20201007</v>
       </c>
@@ -6869,8 +6989,11 @@
       <c r="F282">
         <v>17</v>
       </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G282">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>20201007</v>
       </c>
@@ -6889,8 +7012,11 @@
       <c r="F283">
         <v>18</v>
       </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G283">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>20201007</v>
       </c>
@@ -6909,8 +7035,11 @@
       <c r="F284">
         <v>19</v>
       </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G284">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>20201007</v>
       </c>
@@ -6929,8 +7058,11 @@
       <c r="F285">
         <v>20</v>
       </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G285">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>20201007</v>
       </c>
@@ -6949,8 +7081,11 @@
       <c r="F286">
         <v>21</v>
       </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G286">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>20201007</v>
       </c>
@@ -6969,8 +7104,11 @@
       <c r="F287">
         <v>22</v>
       </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G287">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>20201007</v>
       </c>
@@ -6989,8 +7127,11 @@
       <c r="F288">
         <v>23</v>
       </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G288">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>20201007</v>
       </c>
@@ -7009,8 +7150,11 @@
       <c r="F289">
         <v>24</v>
       </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G289">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>20201007</v>
       </c>
@@ -7029,8 +7173,11 @@
       <c r="F290">
         <v>1</v>
       </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G290">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>20201007</v>
       </c>
@@ -7049,8 +7196,11 @@
       <c r="F291">
         <v>2</v>
       </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G291">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>20201007</v>
       </c>
@@ -7069,8 +7219,11 @@
       <c r="F292">
         <v>3</v>
       </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G292">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>20201007</v>
       </c>
@@ -7089,8 +7242,11 @@
       <c r="F293">
         <v>4</v>
       </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G293">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>20201007</v>
       </c>
@@ -7109,8 +7265,11 @@
       <c r="F294">
         <v>5</v>
       </c>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G294">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>20201007</v>
       </c>
@@ -7129,8 +7288,11 @@
       <c r="F295">
         <v>6</v>
       </c>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G295">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>20201007</v>
       </c>
@@ -7149,8 +7311,11 @@
       <c r="F296">
         <v>7</v>
       </c>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G296">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>20201007</v>
       </c>
@@ -7169,8 +7334,11 @@
       <c r="F297">
         <v>8</v>
       </c>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G297">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>20201007</v>
       </c>
@@ -7189,8 +7357,11 @@
       <c r="F298">
         <v>9</v>
       </c>
-    </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G298">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>20201007</v>
       </c>
@@ -7209,8 +7380,11 @@
       <c r="F299">
         <v>10</v>
       </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G299">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>20201007</v>
       </c>
@@ -7229,8 +7403,11 @@
       <c r="F300">
         <v>11</v>
       </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G300">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>20201007</v>
       </c>
@@ -7249,8 +7426,11 @@
       <c r="F301">
         <v>12</v>
       </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G301">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>20201007</v>
       </c>
@@ -7269,8 +7449,11 @@
       <c r="F302">
         <v>13</v>
       </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G302">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>20201007</v>
       </c>
@@ -7289,8 +7472,11 @@
       <c r="F303">
         <v>14</v>
       </c>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G303">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>20201007</v>
       </c>
@@ -7309,8 +7495,11 @@
       <c r="F304">
         <v>15</v>
       </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G304">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>20201007</v>
       </c>
@@ -7329,8 +7518,11 @@
       <c r="F305">
         <v>16</v>
       </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G305">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>20201007</v>
       </c>
@@ -7349,8 +7541,11 @@
       <c r="F306">
         <v>17</v>
       </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G306">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>20201007</v>
       </c>
@@ -7369,8 +7564,11 @@
       <c r="F307">
         <v>18</v>
       </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G307">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>20201007</v>
       </c>
@@ -7389,8 +7587,11 @@
       <c r="F308">
         <v>19</v>
       </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G308">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>20201007</v>
       </c>
@@ -7409,8 +7610,11 @@
       <c r="F309">
         <v>20</v>
       </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G309">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>20201007</v>
       </c>
@@ -7429,8 +7633,11 @@
       <c r="F310">
         <v>21</v>
       </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G310">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>20201007</v>
       </c>
@@ -7449,8 +7656,11 @@
       <c r="F311">
         <v>22</v>
       </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G311">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>20201007</v>
       </c>
@@ -7469,8 +7679,11 @@
       <c r="F312">
         <v>23</v>
       </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G312">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>20201007</v>
       </c>
@@ -7489,8 +7702,11 @@
       <c r="F313">
         <v>24</v>
       </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G313">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>20201007</v>
       </c>
@@ -7509,8 +7725,11 @@
       <c r="F314">
         <v>1</v>
       </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>20201007</v>
       </c>
@@ -7529,8 +7748,11 @@
       <c r="F315">
         <v>2</v>
       </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>20201007</v>
       </c>
@@ -7549,8 +7771,11 @@
       <c r="F316">
         <v>3</v>
       </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G316">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>20201007</v>
       </c>
@@ -7569,8 +7794,11 @@
       <c r="F317">
         <v>4</v>
       </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G317">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>20201007</v>
       </c>
@@ -7589,8 +7817,11 @@
       <c r="F318">
         <v>5</v>
       </c>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>20201007</v>
       </c>
@@ -7609,8 +7840,11 @@
       <c r="F319">
         <v>6</v>
       </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>20201007</v>
       </c>
@@ -7629,8 +7863,11 @@
       <c r="F320">
         <v>7</v>
       </c>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>20201007</v>
       </c>
@@ -7649,8 +7886,11 @@
       <c r="F321">
         <v>8</v>
       </c>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>20201007</v>
       </c>
@@ -7669,8 +7909,11 @@
       <c r="F322">
         <v>9</v>
       </c>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>20201007</v>
       </c>
@@ -7689,8 +7932,11 @@
       <c r="F323">
         <v>10</v>
       </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>20201007</v>
       </c>
@@ -7709,8 +7955,11 @@
       <c r="F324">
         <v>11</v>
       </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>20201007</v>
       </c>
@@ -7729,8 +7978,11 @@
       <c r="F325">
         <v>12</v>
       </c>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>20201007</v>
       </c>
@@ -7749,8 +8001,11 @@
       <c r="F326">
         <v>13</v>
       </c>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>20201007</v>
       </c>
@@ -7769,8 +8024,11 @@
       <c r="F327">
         <v>14</v>
       </c>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G327">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>20201007</v>
       </c>
@@ -7789,8 +8047,11 @@
       <c r="F328">
         <v>15</v>
       </c>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>20201007</v>
       </c>
@@ -7809,8 +8070,11 @@
       <c r="F329">
         <v>16</v>
       </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>20201007</v>
       </c>
@@ -7829,8 +8093,11 @@
       <c r="F330">
         <v>17</v>
       </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>20201007</v>
       </c>
@@ -7849,8 +8116,11 @@
       <c r="F331">
         <v>18</v>
       </c>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>20201007</v>
       </c>
@@ -7869,8 +8139,11 @@
       <c r="F332">
         <v>19</v>
       </c>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G332">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>20201007</v>
       </c>
@@ -7889,8 +8162,11 @@
       <c r="F333">
         <v>20</v>
       </c>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>20201007</v>
       </c>
@@ -7909,8 +8185,11 @@
       <c r="F334">
         <v>21</v>
       </c>
-    </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>20201007</v>
       </c>
@@ -7929,8 +8208,11 @@
       <c r="F335">
         <v>22</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>20201007</v>
       </c>
@@ -7949,8 +8231,11 @@
       <c r="F336">
         <v>23</v>
       </c>
-    </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>20201007</v>
       </c>
@@ -7969,8 +8254,11 @@
       <c r="F337">
         <v>24</v>
       </c>
-    </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G337">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>20201007</v>
       </c>
@@ -7989,8 +8277,11 @@
       <c r="F338">
         <v>1</v>
       </c>
-    </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G338">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>20201007</v>
       </c>
@@ -8009,8 +8300,11 @@
       <c r="F339">
         <v>2</v>
       </c>
-    </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G339">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>20201007</v>
       </c>
@@ -8029,8 +8323,11 @@
       <c r="F340">
         <v>3</v>
       </c>
-    </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G340">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>20201007</v>
       </c>
@@ -8049,8 +8346,11 @@
       <c r="F341">
         <v>4</v>
       </c>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G341">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>20201007</v>
       </c>
@@ -8069,8 +8369,11 @@
       <c r="F342">
         <v>5</v>
       </c>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G342">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>20201007</v>
       </c>
@@ -8089,8 +8392,11 @@
       <c r="F343">
         <v>6</v>
       </c>
-    </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G343">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>20201007</v>
       </c>
@@ -8109,8 +8415,11 @@
       <c r="F344">
         <v>7</v>
       </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G344">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>20201007</v>
       </c>
@@ -8129,8 +8438,11 @@
       <c r="F345">
         <v>8</v>
       </c>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G345">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>20201007</v>
       </c>
@@ -8149,8 +8461,11 @@
       <c r="F346">
         <v>9</v>
       </c>
-    </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G346">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>20201007</v>
       </c>
@@ -8169,8 +8484,11 @@
       <c r="F347">
         <v>10</v>
       </c>
-    </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G347">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>20201007</v>
       </c>
@@ -8189,8 +8507,11 @@
       <c r="F348">
         <v>11</v>
       </c>
-    </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G348">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>20201007</v>
       </c>
@@ -8209,8 +8530,11 @@
       <c r="F349">
         <v>12</v>
       </c>
-    </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G349">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>20201007</v>
       </c>
@@ -8229,8 +8553,11 @@
       <c r="F350">
         <v>13</v>
       </c>
-    </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G350">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>20201007</v>
       </c>
@@ -8249,8 +8576,11 @@
       <c r="F351">
         <v>14</v>
       </c>
-    </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G351">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>20201007</v>
       </c>
@@ -8269,8 +8599,11 @@
       <c r="F352">
         <v>15</v>
       </c>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G352">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>20201007</v>
       </c>
@@ -8289,8 +8622,11 @@
       <c r="F353">
         <v>16</v>
       </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G353">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>20201007</v>
       </c>
@@ -8309,8 +8645,11 @@
       <c r="F354">
         <v>17</v>
       </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G354">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>20201007</v>
       </c>
@@ -8329,8 +8668,11 @@
       <c r="F355">
         <v>18</v>
       </c>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G355">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>20201007</v>
       </c>
@@ -8349,8 +8691,11 @@
       <c r="F356">
         <v>19</v>
       </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G356">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>20201007</v>
       </c>
@@ -8369,8 +8714,11 @@
       <c r="F357">
         <v>20</v>
       </c>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G357">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>20201007</v>
       </c>
@@ -8389,8 +8737,11 @@
       <c r="F358">
         <v>21</v>
       </c>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G358">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>20201007</v>
       </c>
@@ -8409,8 +8760,11 @@
       <c r="F359">
         <v>22</v>
       </c>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G359">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>20201007</v>
       </c>
@@ -8429,8 +8783,11 @@
       <c r="F360">
         <v>23</v>
       </c>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G360">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>20201007</v>
       </c>
@@ -8449,8 +8806,11 @@
       <c r="F361">
         <v>24</v>
       </c>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G361">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>20201007</v>
       </c>
@@ -8469,8 +8829,11 @@
       <c r="F362">
         <v>1</v>
       </c>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G362">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>20201007</v>
       </c>
@@ -8489,8 +8852,11 @@
       <c r="F363">
         <v>2</v>
       </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G363">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>20201007</v>
       </c>
@@ -8509,8 +8875,11 @@
       <c r="F364">
         <v>3</v>
       </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G364">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>20201007</v>
       </c>
@@ -8529,8 +8898,11 @@
       <c r="F365">
         <v>4</v>
       </c>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G365">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>20201007</v>
       </c>
@@ -8549,8 +8921,11 @@
       <c r="F366">
         <v>5</v>
       </c>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G366">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>20201007</v>
       </c>
@@ -8569,8 +8944,11 @@
       <c r="F367">
         <v>6</v>
       </c>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G367">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>20201007</v>
       </c>
@@ -8589,8 +8967,11 @@
       <c r="F368">
         <v>7</v>
       </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G368">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>20201007</v>
       </c>
@@ -8609,8 +8990,11 @@
       <c r="F369">
         <v>8</v>
       </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G369">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>20201007</v>
       </c>
@@ -8629,8 +9013,11 @@
       <c r="F370">
         <v>9</v>
       </c>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G370">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>20201007</v>
       </c>
@@ -8649,8 +9036,11 @@
       <c r="F371">
         <v>10</v>
       </c>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G371">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>20201007</v>
       </c>
@@ -8669,8 +9059,11 @@
       <c r="F372">
         <v>11</v>
       </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G372">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>20201007</v>
       </c>
@@ -8689,8 +9082,11 @@
       <c r="F373">
         <v>12</v>
       </c>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G373">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>20201007</v>
       </c>
@@ -8709,8 +9105,11 @@
       <c r="F374">
         <v>13</v>
       </c>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G374">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>20201007</v>
       </c>
@@ -8729,8 +9128,11 @@
       <c r="F375">
         <v>14</v>
       </c>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G375">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>20201007</v>
       </c>
@@ -8749,8 +9151,11 @@
       <c r="F376">
         <v>15</v>
       </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G376">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>20201007</v>
       </c>
@@ -8769,8 +9174,11 @@
       <c r="F377">
         <v>16</v>
       </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G377">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>20201007</v>
       </c>
@@ -8789,8 +9197,11 @@
       <c r="F378">
         <v>17</v>
       </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G378">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>20201007</v>
       </c>
@@ -8809,8 +9220,11 @@
       <c r="F379">
         <v>18</v>
       </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G379">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>20201007</v>
       </c>
@@ -8829,8 +9243,11 @@
       <c r="F380">
         <v>19</v>
       </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G380">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>20201007</v>
       </c>
@@ -8849,8 +9266,11 @@
       <c r="F381">
         <v>20</v>
       </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G381">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>20201007</v>
       </c>
@@ -8869,8 +9289,11 @@
       <c r="F382">
         <v>21</v>
       </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G382">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>20201007</v>
       </c>
@@ -8889,8 +9312,11 @@
       <c r="F383">
         <v>22</v>
       </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G383">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>20201007</v>
       </c>
@@ -8909,8 +9335,11 @@
       <c r="F384">
         <v>23</v>
       </c>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G384">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>20201007</v>
       </c>
@@ -8928,6 +9357,9 @@
       </c>
       <c r="F385">
         <v>24</v>
+      </c>
+      <c r="G385">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>